<commit_message>
move heatshield into production
</commit_message>
<xml_diff>
--- a/Source/CalcsAndModels/Heatshields.xlsx
+++ b/Source/CalcsAndModels/Heatshields.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>0625_Heatshield</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t>abl/area</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:O8"/>
+  <dimension ref="B1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -401,7 +404,7 @@
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:17">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -423,6 +426,9 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
       <c r="K1" t="s">
         <v>3</v>
       </c>
@@ -432,8 +438,17 @@
       <c r="M1" t="s">
         <v>5</v>
       </c>
+      <c r="O1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:17">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -461,18 +476,30 @@
       </c>
       <c r="K2">
         <f>F2/$C2^K$8</f>
-        <v>81.92</v>
+        <v>92.134002719186796</v>
       </c>
       <c r="L2">
         <f>G2/$C2^L$8</f>
-        <v>102.4</v>
+        <v>115.1675033989835</v>
       </c>
       <c r="M2">
         <f>H2*$C2^M$8</f>
-        <v>166.71369469114902</v>
+        <v>187.5</v>
+      </c>
+      <c r="O2">
+        <f>F2/$E2</f>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="P2">
+        <f>G2/$E2</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Q2">
+        <f>H2*$E2</f>
+        <v>28800</v>
       </c>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:17">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -500,18 +527,30 @@
       </c>
       <c r="K3">
         <f t="shared" ref="K3:L5" si="0">F3/$C3^K$8</f>
-        <v>40.96</v>
+        <v>38.73757630477008</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>51.2</v>
+        <v>48.421970380962605</v>
       </c>
       <c r="M3">
         <f>H3*$C3^M$8</f>
-        <v>594.77133568531724</v>
+        <v>562.5</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O5" si="1">F3/$E3</f>
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="2">G3/$E3</f>
+        <v>0.32</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q5" si="3">H3*$E3</f>
+        <v>90000</v>
       </c>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:17">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -539,18 +578,30 @@
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>51.2</v>
+        <v>40.717861312872984</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>50.897326641091226</v>
       </c>
       <c r="M4">
         <f>H4*$C4^M$8</f>
-        <v>707.30630419665135</v>
+        <v>562.5</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>0.32</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="3"/>
+        <v>90000</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:17">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -578,50 +629,58 @@
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>91.022222222222226</v>
+        <v>65.409317448924128</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>113.77777777777777</v>
+        <v>81.761646811155146</v>
       </c>
       <c r="M5">
         <f>H5*$C5^M$8</f>
-        <v>450.08878166308159</v>
+        <v>323.4375</v>
       </c>
       <c r="O5">
-        <f>C5^2.75*33</f>
-        <v>1250.5467334340162</v>
+        <f t="shared" si="1"/>
+        <v>0.32</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="3"/>
+        <v>92000</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:17">
       <c r="J7" t="s">
         <v>12</v>
       </c>
       <c r="K7">
         <f>AVERAGE(K3:K5)</f>
-        <v>61.060740740740734</v>
+        <v>48.28825168885573</v>
       </c>
       <c r="L7">
         <f>AVERAGE(L3:L5)</f>
-        <v>76.325925925925915</v>
+        <v>60.360314611069661</v>
       </c>
       <c r="M7">
         <f>AVERAGE(M3:M5)</f>
-        <v>584.05547384835006</v>
+        <v>482.8125</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:17">
       <c r="J8" t="s">
         <v>11</v>
       </c>
       <c r="K8">
+        <v>2.25</v>
+      </c>
+      <c r="L8">
+        <v>2.25</v>
+      </c>
+      <c r="M8">
         <v>2</v>
-      </c>
-      <c r="L8">
-        <v>2</v>
-      </c>
-      <c r="M8">
-        <v>2.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>